<commit_message>
Addin new checklist items
</commit_message>
<xml_diff>
--- a/Checklist/Checklist.xlsx
+++ b/Checklist/Checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\QA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5d3688df6b8265ad/Документы/STOLNIK/Checklist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8E4BD0-DEA3-4F5C-8433-F71DA80091CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E01F4727-B659-4BDE-BCD4-D29DF8BDD4D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4A5DBBCE-3B06-454D-8EB4-AE145C659660}"/>
+    <workbookView xWindow="10845" yWindow="3825" windowWidth="13230" windowHeight="11460" xr2:uid="{4A5DBBCE-3B06-454D-8EB4-AE145C659660}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Анатолий Желтухин</author>
+  </authors>
+  <commentList>
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{FAB24F8E-BB30-4BED-9746-9269657E8893}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Анатолий Желтухин:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+Все тестовые данные вводить на странице https://stolnik24.ru/catalog/zhenskaya-odezhda/</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -54,21 +90,12 @@
     <t>Применить все фильтры одновременно</t>
   </si>
   <si>
-    <t>Черный</t>
-  </si>
-  <si>
-    <t>Весна</t>
-  </si>
-  <si>
     <t>Увеличить UI сайта</t>
   </si>
   <si>
     <t>Уменьшить UI сайта</t>
   </si>
   <si>
-    <t xml:space="preserve"> Увеличить до 200%. Bug - При увеличении UI до 200% пропадает nav bar справа вверху.</t>
-  </si>
-  <si>
     <t>Уменшить до 50%</t>
   </si>
   <si>
@@ -84,9 +111,6 @@
     <t>Уменшить ширину до 600px. Bug - При уменьшении ширины сайта до 985px меню выбора фильтров пропадает</t>
   </si>
   <si>
-    <t>Применить фильтр в поле "Цена"</t>
-  </si>
-  <si>
     <t>Применить фильтр в поле "Цвет"</t>
   </si>
   <si>
@@ -129,9 +153,6 @@
     <t>Добавление в корзину</t>
   </si>
   <si>
-    <t>Выбрать любой товар - размер/цвет - добавить в корзину. Bug - Ничего не происходит, товар не добавляется в корзину</t>
-  </si>
-  <si>
     <t>Добавить минимальное количество товара в корзину</t>
   </si>
   <si>
@@ -159,32 +180,500 @@
     <t>Ввод в текстовое поле поиска отрицательное числовое значение</t>
   </si>
   <si>
-    <t>Туфли</t>
-  </si>
-  <si>
     <t>Ввод в текстовое поле поиска наименование товара на английском</t>
   </si>
   <si>
-    <t>от 399 до 399. Bug - При выборе двух минимальных или максимальных значений фильтра "Цена" (от 399 до 399; от 1299 до 1299) поле и ползунок становятся неактивными. На главном экране так же не отображается товар с примененными фильтрами</t>
-  </si>
-  <si>
     <t>Добавление в корзину не заходя в карточку товара</t>
   </si>
   <si>
     <t xml:space="preserve">Ввод цифр в текстовое поле поиска </t>
   </si>
   <si>
-    <t>Текст: "Цена". Improvment - в поле фильтра "Цена" вводится текст, но не применяется. Лучше ограничить ввод текста и оставить только ввод числовых значений.</t>
-  </si>
-  <si>
-    <t>a</t>
+    <t>Ввод в текстовое поле поиска дробное число</t>
+  </si>
+  <si>
+    <t>Ввод большого количества символов</t>
+  </si>
+  <si>
+    <t>Оставить поле пустым</t>
+  </si>
+  <si>
+    <t>Ввод пробела</t>
+  </si>
+  <si>
+    <t>Ввод максимальных значений в поле "Цена"</t>
+  </si>
+  <si>
+    <t>Ввод отрицательного значения в поле "Цена"</t>
+  </si>
+  <si>
+    <t>Применить минимальную/максимальную фильтрацию в поле "Цена"</t>
+  </si>
+  <si>
+    <t>Ввод среднего значения в поле "Цена"</t>
+  </si>
+  <si>
+    <t>Сохранение фильтров при переходе глубже по дереву</t>
+  </si>
+  <si>
+    <t>Переход на страницу с примененными фильтрами по ссылке</t>
+  </si>
+  <si>
+    <t>Сбросить все параметры фильтрации</t>
+  </si>
+  <si>
+    <t>Фильтр не создает излишних SQL-запросов.</t>
+  </si>
+  <si>
+    <t>Поля содержат только те элементы, по которым могут быть найдены позиции.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>Test data:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Поле "Цена" от 10 до 755. "Цвет" первый в палитре. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Comment: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>Неактивные кнопки стали серыми</t>
+    </r>
+  </si>
+  <si>
+    <t>Увеличить до 200%. Bug - При увеличении UI до 200% пропадает nav bar справа вверху.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Test data: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>от 1000 до 2000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Test data: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>от 399 до 399. Bug - При выборе двух минимальных или максимальных значений фильтра "Цена" (от 399 до 399; от 1299 до 1299) поле и ползунок становятся неактивными. На главном экране так же не отображается товар с примененными фильтрами</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>Test data:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Черный</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Test data: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>26</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Test data: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>Весна</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Test data: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">"Цена". Improvment - в поле фильтра "Цена" вводится текст, но не применяется. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>Comment:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Лучше ограничить ввод текста и оставить только ввод числовых значений.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Test data: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>500000000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>Test data:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> -1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Выбрать любой товар - размер/цвет - добавить в корзину. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Bug </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Ничего не происходит, товар не добавляется в корзину</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Фильтры не сохраняются. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>Improvment - Рекомендую сделать сохранение фильтров</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>Фильтры не сохраняются.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Improvment - Рекомендую сделать сохранение фильтров при переходе "Назад"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Test data: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>123</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Test data: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>Туфли</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Test data: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>-123</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Test data: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>0,5. При вводе дробного числа в  поле поиска выдает неверный результат</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Test data: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>Black</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>Test data:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttest. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Bug: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>При вводе большого количества символов результат запросы выходит за рамки интерфейса сайта</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,6 +694,21 @@
       <color theme="1"/>
       <name val="Segoe UI Emoji"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="4">
@@ -291,7 +795,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -330,6 +834,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -645,11 +1152,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8892CB8C-0601-4C07-8A80-E9519929882A}">
-  <dimension ref="A6:D37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8892CB8C-0601-4C07-8A80-E9519929882A}">
+  <dimension ref="A6:D70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,170 +1181,182 @@
     </row>
     <row r="7" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
     </row>
     <row r="8" spans="2:4" ht="66" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="66" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="12"/>
     </row>
     <row r="12" spans="2:4" ht="33" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="12"/>
     </row>
-    <row r="14" spans="2:4" ht="165" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="8" t="s">
+    <row r="14" spans="2:4" ht="33" x14ac:dyDescent="0.25">
+      <c r="B14" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="33" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>4</v>
-      </c>
       <c r="D15" s="4" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="33" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="4">
-        <v>26</v>
+      <c r="D16" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="33" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="99" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="33" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="33" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
+      <c r="D19" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="33" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="21" spans="2:4" ht="33" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="2:4" ht="33" x14ac:dyDescent="0.25">
+      <c r="D21" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="66" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="2:4" ht="33" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="4"/>
+        <v>48</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="24" spans="2:4" ht="33" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>4</v>
@@ -846,45 +1365,43 @@
     </row>
     <row r="25" spans="2:4" ht="33" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B26" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="12"/>
-    </row>
-    <row r="27" spans="2:4" ht="82.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="33" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" ht="33" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" ht="49.5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B28" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="12"/>
+    </row>
+    <row r="29" spans="2:4" ht="33" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>4</v>
@@ -893,7 +1410,7 @@
     </row>
     <row r="30" spans="2:4" ht="33" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>4</v>
@@ -902,7 +1419,7 @@
     </row>
     <row r="31" spans="2:4" ht="33" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>4</v>
@@ -911,73 +1428,273 @@
     </row>
     <row r="32" spans="2:4" ht="33" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="2:4" ht="33" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B34" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="11"/>
+      <c r="D34" s="12"/>
+    </row>
+    <row r="35" spans="2:4" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B33" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="12"/>
-    </row>
-    <row r="34" spans="2:4" ht="33" x14ac:dyDescent="0.25">
-      <c r="B34" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="4">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" ht="33" x14ac:dyDescent="0.25">
-      <c r="B35" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>4</v>
+      <c r="C35" s="8" t="s">
+        <v>3</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="49.5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="33" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="4">
-        <v>-123</v>
+      <c r="D36" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="2:4" ht="33" x14ac:dyDescent="0.25">
+      <c r="B38" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="2:4" ht="33" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="2:4" ht="33" x14ac:dyDescent="0.25">
+      <c r="B40" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B41" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="11"/>
+      <c r="D41" s="12"/>
+    </row>
+    <row r="42" spans="2:4" ht="33" x14ac:dyDescent="0.25">
+      <c r="B42" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="33" x14ac:dyDescent="0.25">
+      <c r="B43" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="B44" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="B45" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="B46" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" ht="181.5" x14ac:dyDescent="0.25">
+      <c r="B47" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B48" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="4"/>
+    </row>
+    <row r="49" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B49" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="C49" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="4"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50"/>
+      <c r="C50"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51"/>
+      <c r="C51"/>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52"/>
+      <c r="C52"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53"/>
+      <c r="C53"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54"/>
+      <c r="C54"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55"/>
+      <c r="C55"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56"/>
+      <c r="C56"/>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57"/>
+      <c r="C57"/>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58"/>
+      <c r="C58"/>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59"/>
+      <c r="C59"/>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60"/>
+      <c r="C60"/>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61"/>
+      <c r="C61"/>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62"/>
+      <c r="C62"/>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63"/>
+      <c r="C63"/>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64"/>
+      <c r="C64"/>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65"/>
+      <c r="C65"/>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66"/>
+      <c r="C66"/>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67"/>
+      <c r="C67"/>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68"/>
+      <c r="C68"/>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69"/>
+      <c r="C69"/>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B70"/>
+      <c r="C70"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B33:D33"/>
+  <mergeCells count="6">
+    <mergeCell ref="B41:D41"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B28:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>